<commit_message>
Reviewed system measurements polyfit in MATLAB
</commit_message>
<xml_diff>
--- a/Lab3/Medições do Sistema.xlsx
+++ b/Lab3/Medições do Sistema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loure\Dropbox\Lourenço\Faculdade\5A1S\SCDTR\SCDTR-Project\Lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE0559A-6232-404D-99DE-D187A38D3AF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45666F84-2A69-41FB-9322-D1B69619DD0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{94E0B860-0D7F-4EAE-AF2A-5E89F4BDE1C2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>ui</t>
   </si>
@@ -97,6 +97,33 @@
   <si>
     <t>K0</t>
   </si>
+  <si>
+    <t>m=-1,4449E-05</t>
+  </si>
+  <si>
+    <t>b=0,0119</t>
+  </si>
+  <si>
+    <t>[MATLAB]</t>
+  </si>
+  <si>
+    <t>m=0,1001</t>
+  </si>
+  <si>
+    <t>b=44,9773</t>
+  </si>
+  <si>
+    <t>b = 0,0237</t>
+  </si>
+  <si>
+    <t>m=-9E-05</t>
+  </si>
+  <si>
+    <t>b=13,3269</t>
+  </si>
+  <si>
+    <t>m=0,1227</t>
+  </si>
 </sst>
 </file>
 
@@ -147,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -170,6 +197,7 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1294,25 +1322,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>43.54457789</c:v>
+                  <c:v>43,54457789</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.46463503</c:v>
+                  <c:v>52,46463503</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59.53931104</c:v>
+                  <c:v>59,53931104</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>63.46612472</c:v>
+                  <c:v>63,46612472</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68.81720779</c:v>
+                  <c:v>68,81720779</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>78.3188322</c:v>
+                  <c:v>78,3188322</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>81.61547702</c:v>
+                  <c:v>81,61547702</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4376,8 +4404,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>796793</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>100235</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4816,10 +4844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B17B447-7BE9-48E8-9D93-BEADF7CA1324}">
-  <dimension ref="A1:AH32"/>
+  <dimension ref="A1:AH45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA16" sqref="AA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4830,6 +4858,7 @@
     <col min="10" max="10" width="8.7265625" customWidth="1"/>
     <col min="11" max="11" width="13" style="2" customWidth="1"/>
     <col min="13" max="13" width="11.1796875" style="2" customWidth="1"/>
+    <col min="27" max="27" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.35">
@@ -5374,6 +5403,24 @@
         <f>B16*(5/G15-1)^(1/B14)</f>
         <v>9.6769026433156533</v>
       </c>
+      <c r="Q15" t="s">
+        <v>24</v>
+      </c>
+      <c r="R15" t="s">
+        <v>25</v>
+      </c>
+      <c r="S15" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -5422,8 +5469,12 @@
         <f>B16*(5/G16-1)^(1/B14)</f>
         <v>21.586467524230663</v>
       </c>
+      <c r="S16" s="9"/>
+      <c r="AA16">
+        <v>-1.449E-5</v>
+      </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C17">
         <v>1.5</v>
       </c>
@@ -5465,7 +5516,7 @@
         <v>34.361668812879849</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C18">
         <v>2</v>
       </c>
@@ -5506,8 +5557,10 @@
         <f>B16*(5/G18-1)^(1/B14)</f>
         <v>51.706520315048927</v>
       </c>
+      <c r="Y18" s="10"/>
+      <c r="AA18" s="10"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C19">
         <v>2.5</v>
       </c>
@@ -5549,7 +5602,7 @@
         <v>69.738798253763875</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C20">
         <v>3</v>
       </c>
@@ -5591,7 +5644,7 @@
         <v>110.01745965519456</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="C21">
         <v>4</v>
       </c>
@@ -5633,13 +5686,36 @@
         <v>157.93357687038579</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="W32" s="9"/>
+    </row>
+    <row r="44" spans="5:17" x14ac:dyDescent="0.35">
+      <c r="E44" t="s">
+        <v>24</v>
+      </c>
+      <c r="F44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" t="s">
+        <v>29</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P44" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="5:17" x14ac:dyDescent="0.35">
+      <c r="F45" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>